<commit_message>
Casting : ajout bouton refresh
</commit_message>
<xml_diff>
--- a/static/c/casting/perles.xlsx
+++ b/static/c/casting/perles.xlsx
@@ -121,7 +121,7 @@
     <t xml:space="preserve">Mâche beaucoup et dit « eum »</t>
   </si>
   <si>
-    <t xml:space="preserve">"de manière naturelle"</t>
+    <t xml:space="preserve">« de manière naturelle »</t>
   </si>
   <si>
     <t xml:space="preserve">Qu'est-ce que ça peut être long le théâtre quand c'est mauvais</t>
@@ -208,13 +208,40 @@
     <t xml:space="preserve">Aussi immobile que ma grand-mère morte</t>
   </si>
   <si>
-    <t xml:space="preserve">"Y a une petite mise en scène" Ah ouais vraiment toute petite !</t>
+    <t xml:space="preserve">« Y a une petite mise en scène. » Ah ouais vraiment toute petite !</t>
   </si>
   <si>
     <t xml:space="preserve">Mal de mer. La fameuse danse de Gilbert Montagné</t>
   </si>
   <si>
-    <t xml:space="preserve">Le 7ème cercle de l'enfer est constitué de diffusion en boucle de scènes de théâtre joués par ces protagonistes</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Le 7</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">e</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Cambria"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> cercle de l'enfer est constitué de diffusion en boucle de scènes de théâtre joués par ces protagonistes</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Rien à tirer</t>
@@ -466,7 +493,7 @@
     <t xml:space="preserve">English a bit yaourt but sympa</t>
   </si>
   <si>
-    <t xml:space="preserve">Atouts : il fait très bien la goutte, petit "putain" quand il oublie son texte</t>
+    <t xml:space="preserve">Atouts : il fait très bien la goutte, petit « putain » quand il oublie son texte</t>
   </si>
   <si>
     <t xml:space="preserve">NC</t>
@@ -512,7 +539,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -558,6 +585,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
       <sz val="11"/>
       <name val="Cambria"/>
       <family val="0"/>
@@ -652,11 +686,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -679,8 +713,8 @@
   </sheetPr>
   <dimension ref="A1:B134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A101" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B113" activeCellId="0" sqref="B113"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A71" activeCellId="0" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1114,7 +1148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="5" t="s">
         <v>64</v>
       </c>

</xml_diff>